<commit_message>
add name space mapping
</commit_message>
<xml_diff>
--- a/ReconstructionAndAnalysis/suppdata/model_namespace_mappings.xlsx
+++ b/ReconstructionAndAnalysis/suppdata/model_namespace_mappings.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\St. Elmo\Dropbox\Research\Writing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\St. Elmo\Dropbox\Research\Writing\iNlan20\iNlan20\ReconstructionAndAnalysis\suppdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2C1ABCC6-EBA6-4893-9B6F-4E85A5898032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F450CEAD-355D-4EEA-BFF5-0A9EEE93EBCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bigg_kegg_metacyc_mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -10912,7 +10922,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11747,11 +11757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E922"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A898" workbookViewId="0">
-      <selection activeCell="A925" sqref="A925"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24642,22 +24652,10 @@
       </c>
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A922" s="1">
-        <f>COUNTBLANK(A2:A921)</f>
-        <v>0</v>
-      </c>
-      <c r="B922" s="1">
-        <f>COUNTBLANK(B2:B921)</f>
-        <v>2</v>
-      </c>
-      <c r="C922" s="1">
-        <f>COUNTBLANK(C2:C921)</f>
-        <v>235</v>
-      </c>
-      <c r="D922" s="1">
-        <f>COUNTBLANK(D2:D921)</f>
-        <v>338</v>
-      </c>
+      <c r="A922" s="1"/>
+      <c r="B922" s="1"/>
+      <c r="C922" s="1"/>
+      <c r="D922" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E921">

</xml_diff>